<commit_message>
change some values.now everything is OK.
</commit_message>
<xml_diff>
--- a/RFPW_V10A/SCH/RFPW_V10A_IMS电源_V1.0.xlsx
+++ b/RFPW_V10A/SCH/RFPW_V10A_IMS电源_V1.0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="104">
   <si>
     <r>
       <t>FileName</t>
@@ -247,15 +247,6 @@
     <t>105K</t>
   </si>
   <si>
-    <t>294K</t>
-  </si>
-  <si>
-    <t>R3,R10,R16,R21</t>
-  </si>
-  <si>
-    <t>5.11K</t>
-  </si>
-  <si>
     <t>309K</t>
   </si>
   <si>
@@ -286,9 +277,6 @@
     <t>C9,C20</t>
   </si>
   <si>
-    <t>C10,C11,C21,C22</t>
-  </si>
-  <si>
     <t>C35,C49</t>
   </si>
   <si>
@@ -322,24 +310,12 @@
     <t>MARK POINT</t>
   </si>
   <si>
-    <t>R1,R4,R7,R9,R13,R19</t>
-  </si>
-  <si>
-    <t>R2,R8</t>
-  </si>
-  <si>
     <t>R5,R11</t>
   </si>
   <si>
     <t>R6,R12</t>
   </si>
   <si>
-    <t>R14,R20</t>
-  </si>
-  <si>
-    <t>14K</t>
-  </si>
-  <si>
     <t>R15,R24</t>
   </si>
   <si>
@@ -355,40 +331,46 @@
     <t>R18,R23</t>
   </si>
   <si>
-    <t>R25,R26,R27,R28</t>
-  </si>
-  <si>
     <t>TP1,TP2,TP4,TP6</t>
   </si>
   <si>
     <t>MSOP-10-PAD</t>
   </si>
   <si>
+    <t>C10,C21</t>
+  </si>
+  <si>
+    <t>0.5pF_50V/NI</t>
+  </si>
+  <si>
+    <t>C11,C22</t>
+  </si>
+  <si>
+    <t>R1,R2,R7,R8,R13,R19</t>
+  </si>
+  <si>
+    <t>100K</t>
+  </si>
+  <si>
+    <t>R3,R10,R14,R16,R20,R21</t>
+  </si>
+  <si>
+    <t>5.1K</t>
+  </si>
+  <si>
+    <t>R4,R9</t>
+  </si>
+  <si>
+    <t>R25,R26</t>
+  </si>
+  <si>
+    <t>196K</t>
+  </si>
+  <si>
+    <t>R27,R28</t>
+  </si>
+  <si>
     <t>不焊接</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>不焊接</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>不焊接</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>需购买</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>需购买</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>需购买</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>需购买</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -396,7 +378,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,16 +445,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,11 +456,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -540,16 +509,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -577,9 +543,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -599,20 +562,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="差" xfId="1" builtinId="27"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="2" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -953,8 +906,8 @@
   </sheetPr>
   <dimension ref="A1:N198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -1020,56 +973,56 @@
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="7" spans="1:14" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="12"/>
+      <c r="I7" s="11"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="17">
+      <c r="A8" s="16">
         <v>1</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="16">
         <v>10</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="17"/>
+      <c r="H8" s="16"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
@@ -1077,16 +1030,16 @@
       <c r="N8" s="8"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
@@ -1094,30 +1047,28 @@
       <c r="N9" s="8"/>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="19">
+      <c r="A10" s="16">
         <v>2</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="16">
         <v>12</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="19" t="s">
-        <v>104</v>
-      </c>
+      <c r="H10" s="16"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
@@ -1125,16 +1076,16 @@
       <c r="N10" s="8"/>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20" t="s">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
@@ -1142,30 +1093,28 @@
       <c r="N11" s="8"/>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="19">
+      <c r="A12" s="16">
         <v>3</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="16">
         <v>8</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="19" t="s">
-        <v>106</v>
-      </c>
+      <c r="H12" s="16"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
@@ -1173,16 +1122,16 @@
       <c r="N12" s="8"/>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20" t="s">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
@@ -1190,28 +1139,28 @@
       <c r="N13" s="8"/>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="16">
+      <c r="A14" s="15">
         <v>4</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="15">
         <v>4</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="16"/>
+      <c r="H14" s="15"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
@@ -1219,28 +1168,28 @@
       <c r="N14" s="8"/>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="16">
+      <c r="A15" s="15">
         <v>5</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="15">
         <v>2</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="16" t="s">
+      <c r="C15" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="16"/>
+      <c r="H15" s="15"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
@@ -1248,28 +1197,30 @@
       <c r="N15" s="8"/>
     </row>
     <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="16">
+      <c r="A16" s="15">
         <v>6</v>
       </c>
-      <c r="B16" s="16">
-        <v>4</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="16" t="s">
+      <c r="B16" s="15">
+        <v>2</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="16"/>
+      <c r="H16" s="15" t="s">
+        <v>103</v>
+      </c>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
@@ -1277,28 +1228,28 @@
       <c r="N16" s="8"/>
     </row>
     <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="16">
+      <c r="A17" s="15">
         <v>7</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="15">
         <v>2</v>
       </c>
-      <c r="C17" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="16" t="s">
+      <c r="C17" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="16"/>
+      <c r="H17" s="15"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
@@ -1306,28 +1257,28 @@
       <c r="N17" s="8"/>
     </row>
     <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="16">
+      <c r="A18" s="15">
         <v>8</v>
       </c>
-      <c r="B18" s="16">
+      <c r="B18" s="15">
         <v>2</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" s="16" t="s">
+      <c r="C18" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G18" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="16"/>
+      <c r="H18" s="15"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
@@ -1335,30 +1286,28 @@
       <c r="N18" s="8"/>
     </row>
     <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="21">
+      <c r="A19" s="15">
         <v>9</v>
       </c>
-      <c r="B19" s="21">
-        <v>4</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="H19" s="21" t="s">
-        <v>107</v>
-      </c>
+      <c r="B19" s="15">
+        <v>2</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="15"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
@@ -1366,24 +1315,28 @@
       <c r="N19" s="8"/>
     </row>
     <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="16">
+      <c r="A20" s="15">
         <v>10</v>
       </c>
-      <c r="B20" s="16">
-        <v>5</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
+      <c r="B20" s="15">
+        <v>4</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" s="15"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
@@ -1391,30 +1344,24 @@
       <c r="N20" s="8"/>
     </row>
     <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="21">
+      <c r="A21" s="15">
         <v>11</v>
       </c>
-      <c r="B21" s="21">
-        <v>2</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" s="21" t="s">
-        <v>106</v>
-      </c>
+      <c r="B21" s="15">
+        <v>5</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
@@ -1422,30 +1369,28 @@
       <c r="N21" s="8"/>
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="21">
+      <c r="A22" s="15">
         <v>12</v>
       </c>
-      <c r="B22" s="21">
+      <c r="B22" s="15">
         <v>2</v>
       </c>
-      <c r="C22" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" s="21" t="s">
+      <c r="C22" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="F22" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="G22" s="21" t="s">
+      <c r="G22" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="H22" s="21" t="s">
-        <v>106</v>
-      </c>
+      <c r="H22" s="15"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
@@ -1453,28 +1398,28 @@
       <c r="N22" s="8"/>
     </row>
     <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="16">
+      <c r="A23" s="15">
         <v>13</v>
       </c>
-      <c r="B23" s="16">
-        <v>1</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23" s="16"/>
+      <c r="B23" s="15">
+        <v>2</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" s="15"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
@@ -1482,28 +1427,28 @@
       <c r="N23" s="8"/>
     </row>
     <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="11">
+      <c r="A24" s="15">
         <v>14</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="15">
+        <v>1</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11" t="s">
-        <v>101</v>
-      </c>
+      <c r="F24" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="15"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
@@ -1511,28 +1456,26 @@
       <c r="N24" s="8"/>
     </row>
     <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="11">
+      <c r="A25" s="15">
         <v>15</v>
       </c>
-      <c r="B25" s="11">
-        <v>2</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11" t="s">
-        <v>102</v>
-      </c>
+      <c r="B25" s="15">
+        <v>4</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
@@ -1540,28 +1483,26 @@
       <c r="N25" s="8"/>
     </row>
     <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="16">
+      <c r="A26" s="15">
         <v>16</v>
       </c>
-      <c r="B26" s="16">
-        <v>6</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" s="16"/>
+      <c r="B26" s="15">
+        <v>2</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
@@ -1569,28 +1510,28 @@
       <c r="N26" s="8"/>
     </row>
     <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="16">
+      <c r="A27" s="15">
         <v>17</v>
       </c>
-      <c r="B27" s="16">
-        <v>2</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E27" s="16" t="s">
+      <c r="B27" s="15">
+        <v>6</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="G27" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="16"/>
+      <c r="H27" s="15"/>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
@@ -1598,28 +1539,28 @@
       <c r="N27" s="8"/>
     </row>
     <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="16">
+      <c r="A28" s="15">
         <v>18</v>
       </c>
-      <c r="B28" s="16">
-        <v>4</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E28" s="16" t="s">
+      <c r="B28" s="15">
+        <v>6</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="F28" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G28" s="16" t="s">
+      <c r="G28" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H28" s="16"/>
+      <c r="H28" s="15"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
@@ -1627,28 +1568,28 @@
       <c r="N28" s="8"/>
     </row>
     <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="16">
+      <c r="A29" s="15">
         <v>19</v>
       </c>
-      <c r="B29" s="16">
+      <c r="B29" s="15">
         <v>2</v>
       </c>
-      <c r="C29" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="16" t="s">
+      <c r="C29" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F29" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G29" s="16" t="s">
+      <c r="G29" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H29" s="16"/>
+      <c r="H29" s="15"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
@@ -1656,28 +1597,28 @@
       <c r="N29" s="8"/>
     </row>
     <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="16">
+      <c r="A30" s="15">
         <v>20</v>
       </c>
-      <c r="B30" s="16">
+      <c r="B30" s="15">
         <v>2</v>
       </c>
-      <c r="C30" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E30" s="16" t="s">
+      <c r="C30" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F30" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G30" s="16" t="s">
+      <c r="G30" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H30" s="16"/>
+      <c r="H30" s="15"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
@@ -1685,28 +1626,28 @@
       <c r="N30" s="8"/>
     </row>
     <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="16">
+      <c r="A31" s="15">
         <v>21</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B31" s="15">
         <v>2</v>
       </c>
-      <c r="C31" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="E31" s="16" t="s">
+      <c r="C31" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="F31" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G31" s="16" t="s">
+      <c r="G31" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H31" s="16"/>
+      <c r="H31" s="15"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
@@ -1714,28 +1655,28 @@
       <c r="N31" s="8"/>
     </row>
     <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="16">
+      <c r="A32" s="15">
         <v>22</v>
       </c>
-      <c r="B32" s="16">
+      <c r="B32" s="15">
         <v>2</v>
       </c>
-      <c r="C32" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E32" s="16" t="s">
+      <c r="C32" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E32" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="16" t="s">
+      <c r="F32" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G32" s="16" t="s">
+      <c r="G32" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H32" s="16"/>
+      <c r="H32" s="15"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
@@ -1743,28 +1684,28 @@
       <c r="N32" s="8"/>
     </row>
     <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="16">
+      <c r="A33" s="15">
         <v>23</v>
       </c>
-      <c r="B33" s="16">
+      <c r="B33" s="15">
         <v>2</v>
       </c>
-      <c r="C33" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="E33" s="16" t="s">
+      <c r="C33" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="F33" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G33" s="16" t="s">
+      <c r="G33" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="16"/>
+      <c r="H33" s="15"/>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
@@ -1772,28 +1713,28 @@
       <c r="N33" s="8"/>
     </row>
     <row r="34" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="16">
+      <c r="A34" s="15">
         <v>24</v>
       </c>
-      <c r="B34" s="16">
+      <c r="B34" s="15">
         <v>2</v>
       </c>
-      <c r="C34" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D34" s="16" t="s">
+      <c r="C34" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E34" s="16" t="s">
+      <c r="E34" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="F34" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G34" s="16" t="s">
+      <c r="G34" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H34" s="16"/>
+      <c r="H34" s="15"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
@@ -1801,28 +1742,28 @@
       <c r="N34" s="8"/>
     </row>
     <row r="35" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="16">
+      <c r="A35" s="15">
         <v>25</v>
       </c>
-      <c r="B35" s="16">
-        <v>4</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" s="16" t="s">
+      <c r="B35" s="15">
+        <v>2</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F35" s="16" t="s">
+      <c r="F35" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G35" s="16" t="s">
+      <c r="G35" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H35" s="16"/>
+      <c r="H35" s="15"/>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
@@ -1830,28 +1771,28 @@
       <c r="N35" s="8"/>
     </row>
     <row r="36" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="11">
+      <c r="A36" s="15">
         <v>26</v>
       </c>
-      <c r="B36" s="11">
-        <v>4</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11" t="s">
-        <v>103</v>
-      </c>
+      <c r="B36" s="15">
+        <v>2</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="15"/>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
@@ -1859,30 +1800,26 @@
       <c r="N36" s="8"/>
     </row>
     <row r="37" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="21">
+      <c r="A37" s="15">
         <v>27</v>
       </c>
-      <c r="B37" s="21">
+      <c r="B37" s="15">
         <v>4</v>
       </c>
-      <c r="C37" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D37" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="E37" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="F37" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="G37" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="H37" s="21" t="s">
-        <v>105</v>
-      </c>
+      <c r="C37" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
@@ -1890,14 +1827,28 @@
       <c r="N37" s="8"/>
     </row>
     <row r="38" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38"/>
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="D38"/>
-      <c r="E38"/>
-      <c r="F38"/>
-      <c r="G38"/>
-      <c r="H38"/>
+      <c r="A38" s="15">
+        <v>28</v>
+      </c>
+      <c r="B38" s="15">
+        <v>4</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H38" s="15"/>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
@@ -2985,14 +2936,14 @@
       <c r="N110" s="8"/>
     </row>
     <row r="111" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A111" s="13"/>
-      <c r="B111" s="13"/>
-      <c r="C111" s="13"/>
-      <c r="D111" s="13"/>
-      <c r="E111" s="13"/>
-      <c r="F111" s="13"/>
-      <c r="G111" s="13"/>
-      <c r="H111" s="13"/>
+      <c r="A111" s="12"/>
+      <c r="B111" s="12"/>
+      <c r="C111" s="12"/>
+      <c r="D111" s="12"/>
+      <c r="E111" s="12"/>
+      <c r="F111" s="12"/>
+      <c r="G111" s="12"/>
+      <c r="H111" s="12"/>
       <c r="J111" s="8"/>
       <c r="K111" s="8"/>
       <c r="L111" s="8"/>
@@ -3000,14 +2951,14 @@
       <c r="N111" s="8"/>
     </row>
     <row r="112" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A112" s="14"/>
-      <c r="B112" s="14"/>
-      <c r="C112" s="14"/>
-      <c r="D112" s="14"/>
-      <c r="E112" s="14"/>
-      <c r="F112" s="14"/>
-      <c r="G112" s="14"/>
-      <c r="H112" s="14"/>
+      <c r="A112" s="13"/>
+      <c r="B112" s="13"/>
+      <c r="C112" s="13"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="13"/>
+      <c r="F112" s="13"/>
+      <c r="G112" s="13"/>
+      <c r="H112" s="13"/>
       <c r="J112" s="8"/>
       <c r="K112" s="8"/>
       <c r="L112" s="8"/>
@@ -3015,14 +2966,14 @@
       <c r="N112" s="8"/>
     </row>
     <row r="113" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A113" s="14"/>
-      <c r="B113" s="14"/>
-      <c r="C113" s="14"/>
-      <c r="D113" s="14"/>
-      <c r="E113" s="14"/>
-      <c r="F113" s="14"/>
-      <c r="G113" s="14"/>
-      <c r="H113" s="14"/>
+      <c r="A113" s="13"/>
+      <c r="B113" s="13"/>
+      <c r="C113" s="13"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="13"/>
+      <c r="F113" s="13"/>
+      <c r="G113" s="13"/>
+      <c r="H113" s="13"/>
       <c r="J113" s="8"/>
       <c r="K113" s="8"/>
       <c r="L113" s="8"/>
@@ -3030,14 +2981,14 @@
       <c r="N113" s="8"/>
     </row>
     <row r="114" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A114" s="14"/>
-      <c r="B114" s="14"/>
-      <c r="C114" s="14"/>
-      <c r="D114" s="14"/>
-      <c r="E114" s="14"/>
-      <c r="F114" s="14"/>
-      <c r="G114" s="14"/>
-      <c r="H114" s="14"/>
+      <c r="A114" s="13"/>
+      <c r="B114" s="13"/>
+      <c r="C114" s="13"/>
+      <c r="D114" s="13"/>
+      <c r="E114" s="13"/>
+      <c r="F114" s="13"/>
+      <c r="G114" s="13"/>
+      <c r="H114" s="13"/>
       <c r="J114" s="8"/>
       <c r="K114" s="8"/>
       <c r="L114" s="8"/>
@@ -3045,14 +2996,14 @@
       <c r="N114" s="8"/>
     </row>
     <row r="115" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A115" s="14"/>
-      <c r="B115" s="14"/>
-      <c r="C115" s="14"/>
-      <c r="D115" s="14"/>
-      <c r="E115" s="14"/>
-      <c r="F115" s="14"/>
-      <c r="G115" s="14"/>
-      <c r="H115" s="14"/>
+      <c r="A115" s="13"/>
+      <c r="B115" s="13"/>
+      <c r="C115" s="13"/>
+      <c r="D115" s="13"/>
+      <c r="E115" s="13"/>
+      <c r="F115" s="13"/>
+      <c r="G115" s="13"/>
+      <c r="H115" s="13"/>
       <c r="J115" s="8"/>
       <c r="K115" s="8"/>
       <c r="L115" s="8"/>
@@ -3060,14 +3011,14 @@
       <c r="N115" s="8"/>
     </row>
     <row r="116" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A116" s="13"/>
-      <c r="B116" s="13"/>
-      <c r="C116" s="13"/>
-      <c r="D116" s="13"/>
-      <c r="E116" s="13"/>
-      <c r="F116" s="13"/>
-      <c r="G116" s="13"/>
-      <c r="H116" s="13"/>
+      <c r="A116" s="12"/>
+      <c r="B116" s="12"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="12"/>
+      <c r="E116" s="12"/>
+      <c r="F116" s="12"/>
+      <c r="G116" s="12"/>
+      <c r="H116" s="12"/>
       <c r="J116" s="8"/>
       <c r="K116" s="8"/>
       <c r="L116" s="8"/>
@@ -3075,14 +3026,14 @@
       <c r="N116" s="8"/>
     </row>
     <row r="117" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A117" s="14"/>
-      <c r="B117" s="14"/>
-      <c r="C117" s="14"/>
-      <c r="D117" s="14"/>
-      <c r="E117" s="14"/>
-      <c r="F117" s="14"/>
-      <c r="G117" s="14"/>
-      <c r="H117" s="14"/>
+      <c r="A117" s="13"/>
+      <c r="B117" s="13"/>
+      <c r="C117" s="13"/>
+      <c r="D117" s="13"/>
+      <c r="E117" s="13"/>
+      <c r="F117" s="13"/>
+      <c r="G117" s="13"/>
+      <c r="H117" s="13"/>
       <c r="J117" s="8"/>
       <c r="K117" s="8"/>
       <c r="L117" s="8"/>
@@ -3090,14 +3041,14 @@
       <c r="N117" s="8"/>
     </row>
     <row r="118" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A118" s="14"/>
-      <c r="B118" s="14"/>
-      <c r="C118" s="14"/>
-      <c r="D118" s="14"/>
-      <c r="E118" s="14"/>
-      <c r="F118" s="14"/>
-      <c r="G118" s="14"/>
-      <c r="H118" s="14"/>
+      <c r="A118" s="13"/>
+      <c r="B118" s="13"/>
+      <c r="C118" s="13"/>
+      <c r="D118" s="13"/>
+      <c r="E118" s="13"/>
+      <c r="F118" s="13"/>
+      <c r="G118" s="13"/>
+      <c r="H118" s="13"/>
       <c r="J118" s="8"/>
       <c r="K118" s="8"/>
       <c r="L118" s="8"/>
@@ -3105,14 +3056,14 @@
       <c r="N118" s="8"/>
     </row>
     <row r="119" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A119" s="14"/>
-      <c r="B119" s="14"/>
-      <c r="C119" s="14"/>
-      <c r="D119" s="14"/>
-      <c r="E119" s="14"/>
-      <c r="F119" s="14"/>
-      <c r="G119" s="14"/>
-      <c r="H119" s="14"/>
+      <c r="A119" s="13"/>
+      <c r="B119" s="13"/>
+      <c r="C119" s="13"/>
+      <c r="D119" s="13"/>
+      <c r="E119" s="13"/>
+      <c r="F119" s="13"/>
+      <c r="G119" s="13"/>
+      <c r="H119" s="13"/>
       <c r="J119" s="8"/>
       <c r="K119" s="8"/>
       <c r="L119" s="8"/>
@@ -3120,14 +3071,14 @@
       <c r="N119" s="8"/>
     </row>
     <row r="120" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A120" s="14"/>
-      <c r="B120" s="14"/>
-      <c r="C120" s="14"/>
-      <c r="D120" s="14"/>
-      <c r="E120" s="14"/>
-      <c r="F120" s="14"/>
-      <c r="G120" s="14"/>
-      <c r="H120" s="14"/>
+      <c r="A120" s="13"/>
+      <c r="B120" s="13"/>
+      <c r="C120" s="13"/>
+      <c r="D120" s="13"/>
+      <c r="E120" s="13"/>
+      <c r="F120" s="13"/>
+      <c r="G120" s="13"/>
+      <c r="H120" s="13"/>
       <c r="J120" s="8"/>
       <c r="K120" s="8"/>
       <c r="L120" s="8"/>
@@ -3135,14 +3086,14 @@
       <c r="N120" s="8"/>
     </row>
     <row r="121" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A121" s="14"/>
-      <c r="B121" s="14"/>
-      <c r="C121" s="14"/>
-      <c r="D121" s="14"/>
-      <c r="E121" s="14"/>
-      <c r="F121" s="14"/>
-      <c r="G121" s="14"/>
-      <c r="H121" s="14"/>
+      <c r="A121" s="13"/>
+      <c r="B121" s="13"/>
+      <c r="C121" s="13"/>
+      <c r="D121" s="13"/>
+      <c r="E121" s="13"/>
+      <c r="F121" s="13"/>
+      <c r="G121" s="13"/>
+      <c r="H121" s="13"/>
       <c r="J121" s="8"/>
       <c r="K121" s="8"/>
       <c r="L121" s="8"/>
@@ -3150,14 +3101,14 @@
       <c r="N121" s="8"/>
     </row>
     <row r="122" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A122" s="14"/>
-      <c r="B122" s="14"/>
-      <c r="C122" s="14"/>
-      <c r="D122" s="14"/>
-      <c r="E122" s="14"/>
-      <c r="F122" s="14"/>
-      <c r="G122" s="14"/>
-      <c r="H122" s="14"/>
+      <c r="A122" s="13"/>
+      <c r="B122" s="13"/>
+      <c r="C122" s="13"/>
+      <c r="D122" s="13"/>
+      <c r="E122" s="13"/>
+      <c r="F122" s="13"/>
+      <c r="G122" s="13"/>
+      <c r="H122" s="13"/>
       <c r="J122" s="8"/>
       <c r="K122" s="8"/>
       <c r="L122" s="8"/>
@@ -3165,14 +3116,14 @@
       <c r="N122" s="8"/>
     </row>
     <row r="123" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A123" s="14"/>
-      <c r="B123" s="14"/>
-      <c r="C123" s="14"/>
-      <c r="D123" s="14"/>
-      <c r="E123" s="14"/>
-      <c r="F123" s="14"/>
-      <c r="G123" s="14"/>
-      <c r="H123" s="14"/>
+      <c r="A123" s="13"/>
+      <c r="B123" s="13"/>
+      <c r="C123" s="13"/>
+      <c r="D123" s="13"/>
+      <c r="E123" s="13"/>
+      <c r="F123" s="13"/>
+      <c r="G123" s="13"/>
+      <c r="H123" s="13"/>
       <c r="J123" s="8"/>
       <c r="K123" s="8"/>
       <c r="L123" s="8"/>
@@ -3180,14 +3131,14 @@
       <c r="N123" s="8"/>
     </row>
     <row r="124" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A124" s="14"/>
-      <c r="B124" s="14"/>
-      <c r="C124" s="14"/>
-      <c r="D124" s="14"/>
-      <c r="E124" s="14"/>
-      <c r="F124" s="14"/>
-      <c r="G124" s="14"/>
-      <c r="H124" s="14"/>
+      <c r="A124" s="13"/>
+      <c r="B124" s="13"/>
+      <c r="C124" s="13"/>
+      <c r="D124" s="13"/>
+      <c r="E124" s="13"/>
+      <c r="F124" s="13"/>
+      <c r="G124" s="13"/>
+      <c r="H124" s="13"/>
       <c r="J124" s="8"/>
       <c r="K124" s="8"/>
       <c r="L124" s="8"/>
@@ -3195,14 +3146,14 @@
       <c r="N124" s="8"/>
     </row>
     <row r="125" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A125" s="14"/>
-      <c r="B125" s="14"/>
-      <c r="C125" s="14"/>
-      <c r="D125" s="14"/>
-      <c r="E125" s="14"/>
-      <c r="F125" s="14"/>
-      <c r="G125" s="14"/>
-      <c r="H125" s="14"/>
+      <c r="A125" s="13"/>
+      <c r="B125" s="13"/>
+      <c r="C125" s="13"/>
+      <c r="D125" s="13"/>
+      <c r="E125" s="13"/>
+      <c r="F125" s="13"/>
+      <c r="G125" s="13"/>
+      <c r="H125" s="13"/>
       <c r="J125" s="8"/>
       <c r="K125" s="8"/>
       <c r="L125" s="8"/>
@@ -3210,14 +3161,14 @@
       <c r="N125" s="8"/>
     </row>
     <row r="126" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A126" s="14"/>
-      <c r="B126" s="14"/>
-      <c r="C126" s="14"/>
-      <c r="D126" s="14"/>
-      <c r="E126" s="14"/>
-      <c r="F126" s="14"/>
-      <c r="G126" s="14"/>
-      <c r="H126" s="14"/>
+      <c r="A126" s="13"/>
+      <c r="B126" s="13"/>
+      <c r="C126" s="13"/>
+      <c r="D126" s="13"/>
+      <c r="E126" s="13"/>
+      <c r="F126" s="13"/>
+      <c r="G126" s="13"/>
+      <c r="H126" s="13"/>
       <c r="J126" s="8"/>
       <c r="K126" s="8"/>
       <c r="L126" s="8"/>
@@ -3225,14 +3176,14 @@
       <c r="N126" s="8"/>
     </row>
     <row r="127" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A127" s="14"/>
-      <c r="B127" s="14"/>
-      <c r="C127" s="14"/>
-      <c r="D127" s="14"/>
-      <c r="E127" s="14"/>
-      <c r="F127" s="14"/>
-      <c r="G127" s="14"/>
-      <c r="H127" s="14"/>
+      <c r="A127" s="13"/>
+      <c r="B127" s="13"/>
+      <c r="C127" s="13"/>
+      <c r="D127" s="13"/>
+      <c r="E127" s="13"/>
+      <c r="F127" s="13"/>
+      <c r="G127" s="13"/>
+      <c r="H127" s="13"/>
       <c r="J127" s="8"/>
       <c r="K127" s="8"/>
       <c r="L127" s="8"/>
@@ -3240,14 +3191,14 @@
       <c r="N127" s="8"/>
     </row>
     <row r="128" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A128" s="14"/>
-      <c r="B128" s="14"/>
-      <c r="C128" s="14"/>
-      <c r="D128" s="14"/>
-      <c r="E128" s="14"/>
-      <c r="F128" s="14"/>
-      <c r="G128" s="14"/>
-      <c r="H128" s="14"/>
+      <c r="A128" s="13"/>
+      <c r="B128" s="13"/>
+      <c r="C128" s="13"/>
+      <c r="D128" s="13"/>
+      <c r="E128" s="13"/>
+      <c r="F128" s="13"/>
+      <c r="G128" s="13"/>
+      <c r="H128" s="13"/>
       <c r="J128" s="8"/>
       <c r="K128" s="8"/>
       <c r="L128" s="8"/>
@@ -3255,14 +3206,14 @@
       <c r="N128" s="8"/>
     </row>
     <row r="129" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A129" s="14"/>
-      <c r="B129" s="14"/>
-      <c r="C129" s="14"/>
-      <c r="D129" s="14"/>
-      <c r="E129" s="14"/>
-      <c r="F129" s="14"/>
-      <c r="G129" s="14"/>
-      <c r="H129" s="14"/>
+      <c r="A129" s="13"/>
+      <c r="B129" s="13"/>
+      <c r="C129" s="13"/>
+      <c r="D129" s="13"/>
+      <c r="E129" s="13"/>
+      <c r="F129" s="13"/>
+      <c r="G129" s="13"/>
+      <c r="H129" s="13"/>
       <c r="J129" s="8"/>
       <c r="K129" s="8"/>
       <c r="L129" s="8"/>
@@ -3270,14 +3221,14 @@
       <c r="N129" s="8"/>
     </row>
     <row r="130" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A130" s="14"/>
-      <c r="B130" s="14"/>
-      <c r="C130" s="14"/>
-      <c r="D130" s="14"/>
-      <c r="E130" s="14"/>
-      <c r="F130" s="14"/>
-      <c r="G130" s="14"/>
-      <c r="H130" s="14"/>
+      <c r="A130" s="13"/>
+      <c r="B130" s="13"/>
+      <c r="C130" s="13"/>
+      <c r="D130" s="13"/>
+      <c r="E130" s="13"/>
+      <c r="F130" s="13"/>
+      <c r="G130" s="13"/>
+      <c r="H130" s="13"/>
       <c r="J130" s="8"/>
       <c r="K130" s="8"/>
       <c r="L130" s="8"/>
@@ -3285,14 +3236,14 @@
       <c r="N130" s="8"/>
     </row>
     <row r="131" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A131" s="14"/>
-      <c r="B131" s="14"/>
-      <c r="C131" s="14"/>
-      <c r="D131" s="14"/>
-      <c r="E131" s="14"/>
-      <c r="F131" s="14"/>
-      <c r="G131" s="14"/>
-      <c r="H131" s="14"/>
+      <c r="A131" s="13"/>
+      <c r="B131" s="13"/>
+      <c r="C131" s="13"/>
+      <c r="D131" s="13"/>
+      <c r="E131" s="13"/>
+      <c r="F131" s="13"/>
+      <c r="G131" s="13"/>
+      <c r="H131" s="13"/>
       <c r="J131" s="8"/>
       <c r="K131" s="8"/>
       <c r="L131" s="8"/>
@@ -3300,14 +3251,14 @@
       <c r="N131" s="8"/>
     </row>
     <row r="132" spans="1:14" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A132" s="14"/>
-      <c r="B132" s="14"/>
-      <c r="C132" s="14"/>
-      <c r="D132" s="14"/>
-      <c r="E132" s="14"/>
-      <c r="F132" s="14"/>
-      <c r="G132" s="14"/>
-      <c r="H132" s="14"/>
+      <c r="A132" s="13"/>
+      <c r="B132" s="13"/>
+      <c r="C132" s="13"/>
+      <c r="D132" s="13"/>
+      <c r="E132" s="13"/>
+      <c r="F132" s="13"/>
+      <c r="G132" s="13"/>
+      <c r="H132" s="13"/>
       <c r="J132" s="8"/>
       <c r="K132" s="8"/>
       <c r="L132" s="8"/>

</xml_diff>